<commit_message>
updated formulas to compute IOP
Image Overlap Percentage is the percentage of overlap between to consecutive frames used in the VO estimates
</commit_message>
<xml_diff>
--- a/overlap_calculator/overlap_percentage.xlsx
+++ b/overlap_calculator/overlap_percentage.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>INPUTS</t>
   </si>
@@ -111,9 +111,6 @@
     <t>img H</t>
   </si>
   <si>
-    <t>overlap percentage</t>
-  </si>
-  <si>
     <t>perc</t>
   </si>
   <si>
@@ -126,13 +123,46 @@
     <t>none</t>
   </si>
   <si>
-    <t>alpha</t>
-  </si>
-  <si>
     <t>rad</t>
   </si>
   <si>
     <t>b overlap</t>
+  </si>
+  <si>
+    <t>IFD</t>
+  </si>
+  <si>
+    <t>0.02m/s</t>
+  </si>
+  <si>
+    <t>0.07m/s</t>
+  </si>
+  <si>
+    <t>SPEED</t>
+  </si>
+  <si>
+    <t>PITCH</t>
+  </si>
+  <si>
+    <t>CAMERA</t>
+  </si>
+  <si>
+    <t>loccam</t>
+  </si>
+  <si>
+    <t>IOP</t>
+  </si>
+  <si>
+    <t>LOCCAM</t>
+  </si>
+  <si>
+    <t>NAVCAM</t>
+  </si>
+  <si>
+    <t>theta</t>
+  </si>
+  <si>
+    <t>l overlap</t>
   </si>
 </sst>
 </file>
@@ -459,19 +489,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -479,7 +510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -504,14 +535,20 @@
       <c r="N2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3">
         <f>h/(COS(PI()/2 -M4-M6/2))</f>
-        <v>0.29334484250065634</v>
+        <v>0.7775309347720244</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -520,19 +557,25 @@
         <v>1</v>
       </c>
       <c r="K3">
-        <v>0.24</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="L3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <v>0.24</v>
+      </c>
+      <c r="Q3">
+        <v>0.63300000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4">
         <f>h/(COS(PI()/2-M4+M6/2))</f>
-        <v>2.3347998551367244</v>
+        <v>6.6043615220865872</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -541,23 +584,26 @@
         <v>6</v>
       </c>
       <c r="K4">
-        <v>30.4</v>
+        <v>30</v>
       </c>
       <c r="L4" t="s">
         <v>7</v>
       </c>
       <c r="M4">
         <f>RADIANS(K4)</f>
-        <v>0.53058009260627614</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.52359877559829882</v>
+      </c>
+      <c r="P4">
+        <v>30.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5">
         <f>2*TAN(M5/2)*B3</f>
-        <v>0.29251268657631568</v>
+        <v>0.77532524753984733</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -576,13 +622,13 @@
         <v>0.92502450355699462</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6">
         <f>2*TAN(M5/2)*B4</f>
-        <v>2.3281765325139738</v>
+        <v>6.5856263756962781</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -601,13 +647,13 @@
         <v>0.85521133347722145</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7">
         <f>SIN(PI()/2+M6/2)/SIN(-M4+PI()/2)*(B4-B3)</f>
-        <v>2.1537571682115848</v>
+        <v>6.1224418397486584</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -616,19 +662,19 @@
         <v>18</v>
       </c>
       <c r="K7">
-        <v>0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8">
         <f>B5</f>
-        <v>0.29251268657631568</v>
+        <v>0.77532524753984733</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -637,19 +683,19 @@
         <v>22</v>
       </c>
       <c r="K8">
-        <v>0.26667000000000002</v>
+        <v>1</v>
       </c>
       <c r="L8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9">
-        <f>B7-K8*K7*K11</f>
-        <v>2.145757068211585</v>
+        <f>MAX(0,B7-K8*K7*K11)</f>
+        <v>6.0524418397486581</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -661,19 +707,19 @@
         <v>1024</v>
       </c>
       <c r="L9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <f>ATAN((B6-B5)/2)</f>
-        <v>0.79423510298075073</v>
+        <v>1.2392833418188975</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J10" t="s">
         <v>25</v>
@@ -682,40 +728,167 @@
         <v>768</v>
       </c>
       <c r="L10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11">
-        <f>B9*TAN(B10)</f>
-        <v>2.1840200429617544</v>
+        <f>B5+2*B12*TAN(B10)/(B4-B3)</f>
+        <v>19.318349516628249</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
       <c r="J11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12">
+        <f>B9/SIN(PI()/2 -B10)</f>
+        <v>18.595776468253923</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>0.03</v>
+      </c>
+      <c r="J24">
+        <v>0.92340458663566416</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>0.06</v>
+      </c>
+      <c r="J25">
+        <v>0.89903374961988936</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26">
+        <f>((B8+B11)*B9/2)/((B5+B6)*B7/2)*100</f>
+        <v>269.85555443781595</v>
+      </c>
+      <c r="C26" t="s">
         <v>26</v>
       </c>
-      <c r="B26">
-        <f>((B8+B11)*B9/2)/((B5+B6)*B7/2)</f>
-        <v>0.94148274674783927</v>
-      </c>
-      <c r="C26" t="s">
-        <v>27</v>
+      <c r="H26">
+        <v>0.1</v>
+      </c>
+      <c r="I26">
+        <v>0.86704400000000004</v>
+      </c>
+      <c r="J26">
+        <v>0.86704400000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <f>K7*K8</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H27">
+        <v>0.2</v>
+      </c>
+      <c r="J27">
+        <v>0.789594989642042</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>0.3</v>
+      </c>
+      <c r="J28">
+        <v>0.71575232521662158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>0.5</v>
+      </c>
+      <c r="J29">
+        <v>0.57888669240552937</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>0.75</v>
+      </c>
+      <c r="J30">
+        <v>0.42809158146619208</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>0.2998375039429973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created IOP calculator in excel
</commit_message>
<xml_diff>
--- a/overlap_calculator/overlap_percentage.xlsx
+++ b/overlap_calculator/overlap_percentage.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>INPUTS</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>l overlap</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -491,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +551,7 @@
       </c>
       <c r="B3">
         <f>h/(COS(PI()/2 -M4-M6/2))</f>
-        <v>0.7775309347720244</v>
+        <v>0.65689082146821431</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -575,7 +578,7 @@
       </c>
       <c r="B4">
         <f>h/(COS(PI()/2-M4+M6/2))</f>
-        <v>6.6043615220865872</v>
+        <v>1.4703453748182296</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -584,14 +587,14 @@
         <v>6</v>
       </c>
       <c r="K4">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="L4" t="s">
         <v>7</v>
       </c>
       <c r="M4">
         <f>RADIANS(K4)</f>
-        <v>0.52359877559829882</v>
+        <v>0.87266462599716477</v>
       </c>
       <c r="P4">
         <v>30.4</v>
@@ -602,8 +605,8 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <f>2*TAN(M5/2)*B3</f>
-        <v>0.77532524753984733</v>
+        <f>2*TAN(M5/2)*B7</f>
+        <v>1.1482989189115591</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -627,8 +630,8 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <f>2*TAN(M5/2)*B4</f>
-        <v>6.5856263756962781</v>
+        <f>2*TAN(M5/2)*(B7+B13)</f>
+        <v>1.3233473679981884</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -653,7 +656,7 @@
       </c>
       <c r="B7">
         <f>SIN(PI()/2+M6/2)/SIN(-M4+PI()/2)*(B4-B3)</f>
-        <v>6.1224418397486584</v>
+        <v>1.1515656618329364</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -674,7 +677,7 @@
       </c>
       <c r="B8">
         <f>B5</f>
-        <v>0.77532524753984733</v>
+        <v>1.1482989189115591</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -695,7 +698,7 @@
       </c>
       <c r="B9">
         <f>MAX(0,B7-K8*K7*K11)</f>
-        <v>6.0524418397486581</v>
+        <v>1.0815656618329363</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -715,8 +718,8 @@
         <v>42</v>
       </c>
       <c r="B10">
-        <f>ATAN((B6-B5)/2)</f>
-        <v>1.2392833418188975</v>
+        <f>ATAN((B6-B5)/2/(B4-B3))</f>
+        <v>0.1071833696884848</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -737,7 +740,7 @@
       </c>
       <c r="B11">
         <f>B5+2*B12*TAN(B10)/(B4-B3)</f>
-        <v>19.318349516628249</v>
+        <v>1.4360679187063368</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -758,9 +761,21 @@
       </c>
       <c r="B12">
         <f>B9/SIN(PI()/2 -B10)</f>
-        <v>18.595776468253923</v>
+        <v>1.0878082018061381</v>
       </c>
       <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13">
+        <f>B3*SIN(PI()/2-M4-M6/2)</f>
+        <v>0.17554643638987774</v>
+      </c>
+      <c r="C13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -829,7 +844,7 @@
       </c>
       <c r="B26">
         <f>((B8+B11)*B9/2)/((B5+B6)*B7/2)*100</f>
-        <v>269.85555443781595</v>
+        <v>98.2046436610092</v>
       </c>
       <c r="C26" t="s">
         <v>26</v>

</xml_diff>